<commit_message>
finished project description (needs a conclusion).  need to refine the budget, finish project planning, add project planning reference to the project description
</commit_message>
<xml_diff>
--- a/NSF_Career Budget_Hanson.xlsx
+++ b/NSF_Career Budget_Hanson.xlsx
@@ -353,7 +353,7 @@
     <numFmt numFmtId="179" formatCode="\$#,##0.00_);[RED]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="180" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -418,11 +418,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -594,7 +589,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -891,10 +886,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="10" fillId="0" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -951,7 +942,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -967,7 +958,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -983,7 +974,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1015,7 +1006,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1027,7 +1018,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1039,7 +1030,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1123,7 +1114,7 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J51" activeCellId="0" sqref="J51"/>
     </sheetView>
   </sheetViews>
@@ -2109,7 +2100,7 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="F36" s="74" t="n">
+      <c r="F36" s="66" t="n">
         <f aca="false">B36*C36*D36</f>
         <v>250</v>
       </c>
@@ -2131,16 +2122,16 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="75" t="s">
+      <c r="A37" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="76" t="n">
+      <c r="B37" s="75" t="n">
         <v>500</v>
       </c>
       <c r="C37" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="77" t="n">
+      <c r="D37" s="76" t="n">
         <v>1</v>
       </c>
       <c r="E37" s="66" t="n">
@@ -2174,8 +2165,8 @@
         <v>65</v>
       </c>
       <c r="B38" s="68"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="79"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="78"/>
       <c r="E38" s="47" t="n">
         <f aca="false">SUM(E32:E37)</f>
         <v>0</v>
@@ -2202,10 +2193,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="80"/>
-      <c r="B39" s="76"/>
+      <c r="A39" s="79"/>
+      <c r="B39" s="75"/>
       <c r="C39" s="73"/>
-      <c r="D39" s="81"/>
+      <c r="D39" s="80"/>
       <c r="E39" s="66"/>
       <c r="F39" s="66"/>
       <c r="G39" s="66"/>
@@ -2214,12 +2205,12 @@
       <c r="J39" s="66"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="82" t="s">
+      <c r="A40" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="83"/>
-      <c r="C40" s="84"/>
-      <c r="D40" s="85"/>
+      <c r="B40" s="82"/>
+      <c r="C40" s="83"/>
+      <c r="D40" s="84"/>
       <c r="E40" s="64"/>
       <c r="F40" s="64"/>
       <c r="G40" s="64"/>
@@ -2228,10 +2219,10 @@
       <c r="J40" s="64"/>
     </row>
     <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="75"/>
-      <c r="B41" s="76"/>
+      <c r="A41" s="74"/>
+      <c r="B41" s="75"/>
       <c r="C41" s="73"/>
-      <c r="D41" s="81"/>
+      <c r="D41" s="80"/>
       <c r="E41" s="66"/>
       <c r="F41" s="66"/>
       <c r="G41" s="66"/>
@@ -2514,10 +2505,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="86"/>
-      <c r="B50" s="87"/>
-      <c r="C50" s="87"/>
-      <c r="D50" s="88"/>
+      <c r="A50" s="85"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="86"/>
+      <c r="D50" s="87"/>
       <c r="E50" s="66"/>
       <c r="F50" s="66"/>
       <c r="G50" s="66"/>
@@ -2526,12 +2517,12 @@
       <c r="J50" s="66"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="89" t="s">
+      <c r="A51" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="90"/>
-      <c r="C51" s="90"/>
-      <c r="D51" s="91"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="90"/>
       <c r="E51" s="47" t="n">
         <f aca="false">E29+E38+E49</f>
         <v>118362</v>
@@ -2556,28 +2547,28 @@
         <f aca="false">J29+J38+J49</f>
         <v>161841.2552</v>
       </c>
-      <c r="K51" s="92"/>
+      <c r="K51" s="91"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="93"/>
-      <c r="B52" s="94"/>
-      <c r="C52" s="94"/>
-      <c r="D52" s="95"/>
-      <c r="E52" s="96"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="96"/>
-      <c r="H52" s="96"/>
-      <c r="I52" s="96"/>
+      <c r="A52" s="92"/>
+      <c r="B52" s="93"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="95"/>
+      <c r="F52" s="95"/>
+      <c r="G52" s="95"/>
+      <c r="H52" s="95"/>
+      <c r="I52" s="95"/>
       <c r="J52" s="58"/>
-      <c r="K52" s="92"/>
+      <c r="K52" s="91"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="89" t="s">
+      <c r="A53" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="90"/>
-      <c r="C53" s="90"/>
-      <c r="D53" s="91"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="90"/>
       <c r="E53" s="47" t="n">
         <f aca="false">E23+E51</f>
         <v>165400.690416</v>
@@ -2602,36 +2593,36 @@
         <f aca="false">SUM(E53:I53)</f>
         <v>406632.489198671</v>
       </c>
-      <c r="K53" s="92"/>
+      <c r="K53" s="91"/>
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="93"/>
-      <c r="B54" s="97" t="s">
+      <c r="A54" s="92"/>
+      <c r="B54" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="97" t="s">
+      <c r="C54" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="95"/>
-      <c r="E54" s="96"/>
-      <c r="F54" s="96"/>
-      <c r="G54" s="96"/>
-      <c r="H54" s="96"/>
-      <c r="I54" s="96"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="95"/>
+      <c r="H54" s="95"/>
+      <c r="I54" s="95"/>
       <c r="J54" s="58"/>
-      <c r="K54" s="92"/>
+      <c r="K54" s="91"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="89" t="s">
+      <c r="A55" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="98" t="n">
+      <c r="B55" s="97" t="n">
         <v>0.557</v>
       </c>
-      <c r="C55" s="99" t="s">
+      <c r="C55" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="91"/>
+      <c r="D55" s="90"/>
       <c r="E55" s="47" t="n">
         <f aca="false">E15*0.557</f>
         <v>25054.21648</v>
@@ -2658,53 +2649,53 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="93"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="94"/>
-      <c r="D56" s="95"/>
-      <c r="E56" s="96"/>
-      <c r="F56" s="96"/>
-      <c r="G56" s="96"/>
-      <c r="H56" s="96"/>
-      <c r="I56" s="96"/>
+      <c r="A56" s="92"/>
+      <c r="B56" s="99"/>
+      <c r="C56" s="93"/>
+      <c r="D56" s="94"/>
+      <c r="E56" s="95"/>
+      <c r="F56" s="95"/>
+      <c r="G56" s="95"/>
+      <c r="H56" s="95"/>
+      <c r="I56" s="95"/>
       <c r="J56" s="58"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="101" t="s">
+      <c r="A57" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="B57" s="102"/>
-      <c r="C57" s="102"/>
-      <c r="D57" s="103"/>
-      <c r="E57" s="104" t="n">
+      <c r="B57" s="101"/>
+      <c r="C57" s="101"/>
+      <c r="D57" s="102"/>
+      <c r="E57" s="103" t="n">
         <f aca="false">E53+E55</f>
         <v>190454.906896</v>
       </c>
-      <c r="F57" s="104" t="n">
+      <c r="F57" s="103" t="n">
         <f aca="false">F53+F55</f>
         <v>85046.76503392</v>
       </c>
-      <c r="G57" s="104" t="n">
+      <c r="G57" s="103" t="n">
         <f aca="false">G53+G55</f>
         <v>90905.4603345984</v>
       </c>
-      <c r="H57" s="104" t="n">
+      <c r="H57" s="103" t="n">
         <f aca="false">H53+H55</f>
         <v>86584.5295412904</v>
       </c>
-      <c r="I57" s="104" t="n">
+      <c r="I57" s="103" t="n">
         <f aca="false">I53+I55</f>
         <v>84023.9761321162</v>
       </c>
-      <c r="J57" s="104" t="n">
+      <c r="J57" s="103" t="n">
         <f aca="false">J53+J55</f>
         <v>537015.637937925</v>
       </c>
-      <c r="K57" s="92"/>
+      <c r="K57" s="91"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="105"/>
-      <c r="D58" s="106"/>
+      <c r="A58" s="104"/>
+      <c r="D58" s="105"/>
       <c r="E58" s="54"/>
       <c r="F58" s="54"/>
       <c r="G58" s="54"/>
@@ -2713,8 +2704,8 @@
       <c r="J58" s="54"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="107"/>
-      <c r="D59" s="106"/>
+      <c r="A59" s="106"/>
+      <c r="D59" s="105"/>
       <c r="E59" s="54"/>
       <c r="F59" s="54"/>
       <c r="G59" s="54"/>
@@ -2753,59 +2744,59 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="110"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
+      <c r="A2" s="109"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="110" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="110" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="110" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="110" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="110" t="n">
+      <c r="C4" s="109" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="110" t="n">
+      <c r="D4" s="109" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="110" t="n">
+      <c r="E4" s="109" t="n">
         <f aca="false">C4*D4</f>
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Created and finished year 3 of project plan, and started year 4.  Budget modifications
</commit_message>
<xml_diff>
--- a/NSF_Career Budget_Hanson.xlsx
+++ b/NSF_Career Budget_Hanson.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
   <si>
     <t xml:space="preserve">CAREER: Translation of Machine Learning and Additive Manufacturing to Accelerate and Diversify Science and Engineering</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t xml:space="preserve">Materials &amp; Supplies: Connectors, cables, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android mobile devices</t>
   </si>
   <si>
     <t xml:space="preserve">Publication/Documentation/Dissemination</t>
@@ -1114,8 +1117,8 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J51" activeCellId="0" sqref="J51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1370,11 +1373,11 @@
         <v>16120</v>
       </c>
       <c r="F11" s="35" t="n">
-        <f aca="false">E11*1.02</f>
-        <v>16442.4</v>
+        <f aca="false">E11*1.02*5/4</f>
+        <v>20553</v>
       </c>
       <c r="G11" s="35" t="n">
-        <f aca="false">F11*1.02</f>
+        <f aca="false">F11*1.02*4/5</f>
         <v>16771.248</v>
       </c>
       <c r="H11" s="35" t="n">
@@ -1387,7 +1390,7 @@
       </c>
       <c r="J11" s="35" t="n">
         <f aca="false">SUM(E11:I11)</f>
-        <v>83889.1273792</v>
+        <v>87999.7273792</v>
       </c>
     </row>
     <row r="12" s="26" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1409,27 +1412,27 @@
         <v>8370</v>
       </c>
       <c r="F12" s="35" t="n">
-        <f aca="false">E12*1.02</f>
-        <v>8537.4</v>
+        <f aca="false">E12*1.02*0.33</f>
+        <v>2817.342</v>
       </c>
       <c r="G12" s="35" t="n">
-        <f aca="false">F12*1.02</f>
-        <v>8708.148</v>
+        <f aca="false">F12*1.02*3</f>
+        <v>8621.06652</v>
       </c>
       <c r="H12" s="35" t="n">
-        <f aca="false">G12*1.02</f>
-        <v>8882.31096</v>
+        <f aca="false">G12*1.02*0.33</f>
+        <v>2901.850990632</v>
       </c>
       <c r="I12" s="35" t="n">
         <f aca="false">H12*1.02</f>
-        <v>9059.9571792</v>
+        <v>2959.88801044464</v>
       </c>
       <c r="J12" s="35" t="n">
         <f aca="false">SUM(E12:I12)</f>
-        <v>43557.8161392</v>
-      </c>
-    </row>
-    <row r="13" s="26" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25670.1475210766</v>
+      </c>
+    </row>
+    <row r="13" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="s">
         <v>35</v>
       </c>
@@ -1511,23 +1514,23 @@
       </c>
       <c r="F15" s="47" t="n">
         <f aca="false">SUM(F8:F14)</f>
-        <v>45880.2528</v>
+        <v>44270.7948</v>
       </c>
       <c r="G15" s="47" t="n">
         <f aca="false">SUM(G8:G14)</f>
-        <v>46797.857856</v>
+        <v>46710.776376</v>
       </c>
       <c r="H15" s="47" t="n">
         <f aca="false">SUM(H8:H14)</f>
-        <v>47733.81501312</v>
+        <v>41753.355043752</v>
       </c>
       <c r="I15" s="47" t="n">
         <f aca="false">SUM(I8:I14)</f>
-        <v>48688.4913133824</v>
+        <v>42588.4221446271</v>
       </c>
       <c r="J15" s="47" t="n">
         <f aca="false">SUM(J8:J14)</f>
-        <v>234081.056982502</v>
+        <v>220303.988364379</v>
       </c>
       <c r="K15" s="48"/>
       <c r="L15" s="48"/>
@@ -1623,7 +1626,7 @@
       </c>
       <c r="F19" s="35" t="n">
         <f aca="false">$B$19*F11</f>
-        <v>54.8189616</v>
+        <v>68.523702</v>
       </c>
       <c r="G19" s="35" t="n">
         <f aca="false">$B$19*G11</f>
@@ -1639,7 +1642,7 @@
       </c>
       <c r="J19" s="35" t="n">
         <f aca="false">SUM(E19:I19)</f>
-        <v>279.686350682253</v>
+        <v>293.391091082253</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,23 +1660,23 @@
       </c>
       <c r="F20" s="35" t="n">
         <f aca="false">F12*$D$20</f>
-        <v>681.28452</v>
+        <v>224.8238916</v>
       </c>
       <c r="G20" s="35" t="n">
         <f aca="false">G12*$D$20</f>
-        <v>694.9102104</v>
+        <v>687.961108296</v>
       </c>
       <c r="H20" s="35" t="n">
         <f aca="false">H12*$D$20</f>
-        <v>708.808414608</v>
+        <v>231.567709052434</v>
       </c>
       <c r="I20" s="35" t="n">
         <f aca="false">I12*$D$20</f>
-        <v>722.98458290016</v>
+        <v>236.199063233482</v>
       </c>
       <c r="J20" s="35" t="n">
         <f aca="false">SUM(E20:I20)</f>
-        <v>3475.91372790816</v>
+        <v>2048.47777218192</v>
       </c>
       <c r="K20" s="54"/>
     </row>
@@ -1690,23 +1693,23 @@
       </c>
       <c r="F21" s="55" t="n">
         <f aca="false">SUM(F17:F20)</f>
-        <v>2099.21142432</v>
+        <v>1656.45553632</v>
       </c>
       <c r="G21" s="55" t="n">
         <f aca="false">SUM(G17:G20)</f>
-        <v>2141.1956528064</v>
+        <v>2134.2465507024</v>
       </c>
       <c r="H21" s="55" t="n">
         <f aca="false">SUM(H17:H20)</f>
-        <v>2184.01956586253</v>
+        <v>1706.77886030696</v>
       </c>
       <c r="I21" s="55" t="n">
         <f aca="false">SUM(I17:I20)</f>
-        <v>2227.69995717978</v>
+        <v>1740.91443751311</v>
       </c>
       <c r="J21" s="55" t="n">
         <f aca="false">SUM(J17:J20)</f>
-        <v>10710.1770161687</v>
+        <v>9296.44580084246</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,23 +1737,23 @@
       </c>
       <c r="F23" s="47" t="n">
         <f aca="false">F15+F21</f>
-        <v>47979.46422432</v>
+        <v>45927.25033632</v>
       </c>
       <c r="G23" s="47" t="n">
         <f aca="false">G15+G21</f>
-        <v>48939.0535088064</v>
+        <v>48845.0229267024</v>
       </c>
       <c r="H23" s="47" t="n">
         <f aca="false">H15+H21</f>
-        <v>49917.8345789825</v>
+        <v>43460.133904059</v>
       </c>
       <c r="I23" s="47" t="n">
         <f aca="false">I15+I21</f>
-        <v>50916.1912705622</v>
+        <v>44329.3365821402</v>
       </c>
       <c r="J23" s="47" t="n">
         <f aca="false">J15+J21</f>
-        <v>244791.233998671</v>
+        <v>229600.434165221</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,11 +1864,12 @@
         <v>8</v>
       </c>
       <c r="E28" s="66" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="66" t="n">
         <f aca="false">B28*D28</f>
         <v>13920</v>
-      </c>
-      <c r="F28" s="66" t="n">
-        <v>0</v>
       </c>
       <c r="G28" s="66" t="n">
         <v>0</v>
@@ -1890,22 +1894,22 @@
       <c r="D29" s="69"/>
       <c r="E29" s="70" t="n">
         <f aca="false">SUM(E26:E28)</f>
-        <v>113920</v>
+        <v>100000</v>
       </c>
       <c r="F29" s="70" t="n">
-        <f aca="false">SUM(F26:F27)</f>
-        <v>0</v>
+        <f aca="false">SUM(F26:F28)</f>
+        <v>13920</v>
       </c>
       <c r="G29" s="70" t="n">
-        <f aca="false">SUM(G26:G27)</f>
+        <f aca="false">SUM(G26:G28)</f>
         <v>0</v>
       </c>
       <c r="H29" s="70" t="n">
-        <f aca="false">SUM(H26:H27)</f>
+        <f aca="false">SUM(H26:H28)</f>
         <v>0</v>
       </c>
       <c r="I29" s="70" t="n">
-        <f aca="false">SUM(I26:I27)</f>
+        <f aca="false">SUM(I26:I28)</f>
         <v>0</v>
       </c>
       <c r="J29" s="70" t="n">
@@ -2371,69 +2375,66 @@
         <v>73</v>
       </c>
       <c r="B46" s="26" t="n">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="C46" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="D46" s="72" t="s">
-        <v>70</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D46" s="72"/>
       <c r="E46" s="66" t="n">
         <v>0</v>
       </c>
       <c r="F46" s="66" t="n">
-        <f aca="false">B46</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="G46" s="66" t="n">
-        <f aca="false">B46</f>
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="H46" s="66" t="n">
         <v>0</v>
       </c>
       <c r="I46" s="66" t="n">
-        <f aca="false">0</f>
         <v>0</v>
       </c>
       <c r="J46" s="66" t="n">
-        <f aca="false">SUM(E46:I46)</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="K46" s="54"/>
     </row>
-    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="27" t="s">
         <v>74</v>
       </c>
       <c r="B47" s="26" t="n">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="C47" s="72" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" s="72" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D47" s="72" t="s">
+        <v>70</v>
       </c>
       <c r="E47" s="66" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F47" s="66" t="n">
-        <v>500</v>
+        <f aca="false">B47</f>
+        <v>2500</v>
       </c>
       <c r="G47" s="66" t="n">
-        <v>500</v>
+        <f aca="false">B47</f>
+        <v>2500</v>
       </c>
       <c r="H47" s="66" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I47" s="66" t="n">
-        <v>500</v>
+        <f aca="false">0</f>
+        <v>0</v>
       </c>
       <c r="J47" s="66" t="n">
         <f aca="false">SUM(E47:I47)</f>
-        <v>2500</v>
+        <v>5000</v>
       </c>
       <c r="K47" s="54"/>
     </row>
@@ -2442,269 +2443,293 @@
         <v>75</v>
       </c>
       <c r="B48" s="26" t="n">
+        <v>500</v>
+      </c>
+      <c r="C48" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="F48" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="G48" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="H48" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="I48" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="J48" s="66" t="n">
+        <f aca="false">SUM(E48:I48)</f>
+        <v>2500</v>
+      </c>
+      <c r="K48" s="54"/>
+    </row>
+    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="26" t="n">
         <f aca="false">450+(2*250)+(3*74)+100</f>
         <v>1272</v>
       </c>
-      <c r="C48" s="72" t="n">
+      <c r="C49" s="72" t="n">
         <v>1</v>
       </c>
-      <c r="D48" s="72" t="n">
+      <c r="D49" s="72" t="n">
         <v>1</v>
       </c>
-      <c r="E48" s="66" t="n">
+      <c r="E49" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="F48" s="66" t="n">
+      <c r="F49" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="G48" s="66" t="n">
+      <c r="G49" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="H48" s="66" t="n">
+      <c r="H49" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="I48" s="66" t="n">
+      <c r="I49" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="J48" s="66" t="n">
-        <f aca="false">SUM(E48:I48)</f>
+      <c r="J49" s="66" t="n">
+        <f aca="false">SUM(E49:I49)</f>
         <v>6360</v>
       </c>
-      <c r="K48" s="54"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="47" t="n">
-        <f aca="false">SUM(E43:E48)</f>
+      <c r="K49" s="54"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="47" t="n">
+        <f aca="false">SUM(E43:E49)</f>
         <v>4442</v>
       </c>
-      <c r="F49" s="47" t="n">
-        <f aca="false">SUM(F43:F48)</f>
+      <c r="F50" s="47" t="n">
+        <f aca="false">SUM(F43:F49)</f>
         <v>9112</v>
       </c>
-      <c r="G49" s="47" t="n">
-        <f aca="false">SUM(G43:G48)</f>
-        <v>13452</v>
-      </c>
-      <c r="H49" s="47" t="n">
-        <f aca="false">SUM(H43:H48)</f>
+      <c r="G50" s="47" t="n">
+        <f aca="false">SUM(G43:G49)</f>
+        <v>15452</v>
+      </c>
+      <c r="H50" s="47" t="n">
+        <f aca="false">SUM(H43:H49)</f>
         <v>7582</v>
       </c>
-      <c r="I49" s="47" t="n">
-        <f aca="false">SUM(I43:I48)</f>
+      <c r="I50" s="47" t="n">
+        <f aca="false">SUM(I43:I49)</f>
         <v>3472</v>
       </c>
-      <c r="J49" s="47" t="n">
-        <f aca="false">SUM(J43:J48)</f>
+      <c r="J50" s="47" t="n">
+        <f aca="false">SUM(J43:J49)</f>
         <v>38060</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="85"/>
-      <c r="B50" s="86"/>
-      <c r="C50" s="86"/>
-      <c r="D50" s="87"/>
-      <c r="E50" s="66"/>
-      <c r="F50" s="66"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-      <c r="J50" s="66"/>
-    </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="88" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="47" t="n">
-        <f aca="false">E29+E38+E49</f>
-        <v>118362</v>
-      </c>
-      <c r="F51" s="47" t="n">
-        <f aca="false">F29+F38+F49</f>
-        <v>11512</v>
-      </c>
-      <c r="G51" s="47" t="n">
-        <f aca="false">G29+G38+G49</f>
-        <v>15900</v>
-      </c>
-      <c r="H51" s="47" t="n">
-        <f aca="false">H29+H38+H49</f>
+      <c r="A51" s="85"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="66"/>
+      <c r="G51" s="66"/>
+      <c r="H51" s="66"/>
+      <c r="I51" s="66"/>
+      <c r="J51" s="66"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="88" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="89"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="90"/>
+      <c r="E52" s="47" t="n">
+        <f aca="false">E29+E38+E50</f>
+        <v>104442</v>
+      </c>
+      <c r="F52" s="47" t="n">
+        <f aca="false">F29+F38+F50</f>
+        <v>25432</v>
+      </c>
+      <c r="G52" s="47" t="n">
+        <f aca="false">G29+G38+G50</f>
+        <v>17900</v>
+      </c>
+      <c r="H52" s="47" t="n">
+        <f aca="false">H29+H38+H50</f>
         <v>10078.96</v>
       </c>
-      <c r="I51" s="47" t="n">
-        <f aca="false">I29+I38+I49</f>
+      <c r="I52" s="47" t="n">
+        <f aca="false">I29+I38+I50</f>
         <v>5988.2952</v>
       </c>
-      <c r="J51" s="47" t="n">
-        <f aca="false">J29+J38+J49</f>
+      <c r="J52" s="47" t="n">
+        <f aca="false">J29+J38+J50</f>
         <v>161841.2552</v>
       </c>
-      <c r="K51" s="91"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="92"/>
-      <c r="B52" s="93"/>
-      <c r="C52" s="93"/>
-      <c r="D52" s="94"/>
-      <c r="E52" s="95"/>
-      <c r="F52" s="95"/>
-      <c r="G52" s="95"/>
-      <c r="H52" s="95"/>
-      <c r="I52" s="95"/>
-      <c r="J52" s="58"/>
       <c r="K52" s="91"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="88" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="89"/>
-      <c r="C53" s="89"/>
-      <c r="D53" s="90"/>
-      <c r="E53" s="47" t="n">
-        <f aca="false">E23+E51</f>
-        <v>165400.690416</v>
-      </c>
-      <c r="F53" s="47" t="n">
-        <f aca="false">F23+F51</f>
-        <v>59491.46422432</v>
-      </c>
-      <c r="G53" s="47" t="n">
-        <f aca="false">G23+G51</f>
-        <v>64839.0535088064</v>
-      </c>
-      <c r="H53" s="47" t="n">
-        <f aca="false">H23+H51</f>
-        <v>59996.7945789825</v>
-      </c>
-      <c r="I53" s="47" t="n">
-        <f aca="false">I23+I51</f>
-        <v>56904.4864705622</v>
-      </c>
-      <c r="J53" s="55" t="n">
-        <f aca="false">SUM(E53:I53)</f>
-        <v>406632.489198671</v>
-      </c>
+      <c r="A53" s="92"/>
+      <c r="B53" s="93"/>
+      <c r="C53" s="93"/>
+      <c r="D53" s="94"/>
+      <c r="E53" s="95"/>
+      <c r="F53" s="95"/>
+      <c r="G53" s="95"/>
+      <c r="H53" s="95"/>
+      <c r="I53" s="95"/>
+      <c r="J53" s="58"/>
       <c r="K53" s="91"/>
     </row>
-    <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="92"/>
-      <c r="B54" s="96" t="s">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="89"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="47" t="n">
+        <f aca="false">E23+E52</f>
+        <v>151480.690416</v>
+      </c>
+      <c r="F54" s="47" t="n">
+        <f aca="false">F23+F52</f>
+        <v>71359.25033632</v>
+      </c>
+      <c r="G54" s="47" t="n">
+        <f aca="false">G23+G52</f>
+        <v>66745.0229267024</v>
+      </c>
+      <c r="H54" s="47" t="n">
+        <f aca="false">H23+H52</f>
+        <v>53539.093904059</v>
+      </c>
+      <c r="I54" s="47" t="n">
+        <f aca="false">I23+I52</f>
+        <v>50317.6317821402</v>
+      </c>
+      <c r="J54" s="55" t="n">
+        <f aca="false">SUM(E54:I54)</f>
+        <v>393441.689365221</v>
+      </c>
+      <c r="K54" s="91"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="92"/>
+      <c r="B55" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="D54" s="94"/>
-      <c r="E54" s="95"/>
-      <c r="F54" s="95"/>
-      <c r="G54" s="95"/>
-      <c r="H54" s="95"/>
-      <c r="I54" s="95"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="91"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="88" t="s">
+      <c r="C55" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="97" t="n">
+      <c r="D55" s="94"/>
+      <c r="E55" s="95"/>
+      <c r="F55" s="95"/>
+      <c r="G55" s="95"/>
+      <c r="H55" s="95"/>
+      <c r="I55" s="95"/>
+      <c r="J55" s="58"/>
+      <c r="K55" s="91"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="88" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="97" t="n">
         <v>0.557</v>
       </c>
-      <c r="C55" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" s="90"/>
-      <c r="E55" s="47" t="n">
+      <c r="C56" s="98" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="90"/>
+      <c r="E56" s="47" t="n">
         <f aca="false">E15*0.557</f>
         <v>25054.21648</v>
       </c>
-      <c r="F55" s="47" t="n">
+      <c r="F56" s="47" t="n">
         <f aca="false">F15*0.557</f>
-        <v>25555.3008096</v>
-      </c>
-      <c r="G55" s="47" t="n">
+        <v>24658.8327036</v>
+      </c>
+      <c r="G56" s="47" t="n">
         <f aca="false">G15*0.557</f>
-        <v>26066.406825792</v>
-      </c>
-      <c r="H55" s="47" t="n">
+        <v>26017.902441432</v>
+      </c>
+      <c r="H56" s="47" t="n">
         <f aca="false">H15*0.557</f>
-        <v>26587.7349623078</v>
-      </c>
-      <c r="I55" s="47" t="n">
+        <v>23256.6187593699</v>
+      </c>
+      <c r="I56" s="47" t="n">
         <f aca="false">I15*0.557</f>
-        <v>27119.489661554</v>
-      </c>
-      <c r="J55" s="55" t="n">
-        <f aca="false">SUM(E55:I55)</f>
-        <v>130383.148739254</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="92"/>
-      <c r="B56" s="99"/>
-      <c r="C56" s="93"/>
-      <c r="D56" s="94"/>
-      <c r="E56" s="95"/>
-      <c r="F56" s="95"/>
-      <c r="G56" s="95"/>
-      <c r="H56" s="95"/>
-      <c r="I56" s="95"/>
-      <c r="J56" s="58"/>
+        <v>23721.7511345573</v>
+      </c>
+      <c r="J56" s="55" t="n">
+        <f aca="false">SUM(E56:I56)</f>
+        <v>122709.321518959</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="100" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57" s="101"/>
-      <c r="C57" s="101"/>
-      <c r="D57" s="102"/>
-      <c r="E57" s="103" t="n">
-        <f aca="false">E53+E55</f>
-        <v>190454.906896</v>
-      </c>
-      <c r="F57" s="103" t="n">
-        <f aca="false">F53+F55</f>
-        <v>85046.76503392</v>
-      </c>
-      <c r="G57" s="103" t="n">
-        <f aca="false">G53+G55</f>
-        <v>90905.4603345984</v>
-      </c>
-      <c r="H57" s="103" t="n">
-        <f aca="false">H53+H55</f>
-        <v>86584.5295412904</v>
-      </c>
-      <c r="I57" s="103" t="n">
-        <f aca="false">I53+I55</f>
-        <v>84023.9761321162</v>
-      </c>
-      <c r="J57" s="103" t="n">
-        <f aca="false">J53+J55</f>
-        <v>537015.637937925</v>
-      </c>
-      <c r="K57" s="91"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="104"/>
-      <c r="D58" s="105"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
-      <c r="I58" s="54"/>
-      <c r="J58" s="54"/>
+      <c r="A57" s="92"/>
+      <c r="B57" s="99"/>
+      <c r="C57" s="93"/>
+      <c r="D57" s="94"/>
+      <c r="E57" s="95"/>
+      <c r="F57" s="95"/>
+      <c r="G57" s="95"/>
+      <c r="H57" s="95"/>
+      <c r="I57" s="95"/>
+      <c r="J57" s="58"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="100" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="101"/>
+      <c r="C58" s="101"/>
+      <c r="D58" s="102"/>
+      <c r="E58" s="103" t="n">
+        <f aca="false">E54+E56</f>
+        <v>176534.906896</v>
+      </c>
+      <c r="F58" s="103" t="n">
+        <f aca="false">F54+F56</f>
+        <v>96018.08303992</v>
+      </c>
+      <c r="G58" s="103" t="n">
+        <f aca="false">G54+G56</f>
+        <v>92762.9253681344</v>
+      </c>
+      <c r="H58" s="103" t="n">
+        <f aca="false">H54+H56</f>
+        <v>76795.7126634288</v>
+      </c>
+      <c r="I58" s="103" t="n">
+        <f aca="false">I54+I56</f>
+        <v>74039.3829166974</v>
+      </c>
+      <c r="J58" s="103" t="n">
+        <f aca="false">J54+J56</f>
+        <v>516151.010884181</v>
+      </c>
+      <c r="K58" s="91"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="106"/>
+      <c r="A59" s="104"/>
       <c r="D59" s="105"/>
       <c r="E59" s="54"/>
       <c r="F59" s="54"/>
@@ -2713,7 +2738,16 @@
       <c r="I59" s="54"/>
       <c r="J59" s="54"/>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="106"/>
+      <c r="D60" s="105"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
+      <c r="I60" s="54"/>
+      <c r="J60" s="54"/>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -2744,7 +2778,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
@@ -2752,7 +2786,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="107" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="109"/>
@@ -2768,24 +2802,24 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="110" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B3" s="110" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="110" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="110" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" s="110" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="109" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B4" s="108" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
updating project plans and budget
</commit_message>
<xml_diff>
--- a/NSF_Career Budget_Hanson.xlsx
+++ b/NSF_Career Budget_Hanson.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t xml:space="preserve">CAREER: Translation of Machine Learning and Additive Manufacturing to Accelerate and Diversify Science and Engineering</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t xml:space="preserve">Android mobile devices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drone parts</t>
   </si>
   <si>
     <t xml:space="preserve">Publication/Documentation/Dissemination</t>
@@ -1118,7 +1121,7 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1381,16 +1384,16 @@
         <v>16771.248</v>
       </c>
       <c r="H11" s="35" t="n">
-        <f aca="false">G11*1.02</f>
-        <v>17106.67296</v>
+        <f aca="false">G11*1.02*2/4</f>
+        <v>8553.33648</v>
       </c>
       <c r="I11" s="35" t="n">
-        <f aca="false">H11*1.02</f>
+        <f aca="false">H11*1.02*4/2</f>
         <v>17448.8064192</v>
       </c>
       <c r="J11" s="35" t="n">
         <f aca="false">SUM(E11:I11)</f>
-        <v>87999.7273792</v>
+        <v>79446.3908992</v>
       </c>
     </row>
     <row r="12" s="26" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1525,7 @@
       </c>
       <c r="H15" s="47" t="n">
         <f aca="false">SUM(H8:H14)</f>
-        <v>41753.355043752</v>
+        <v>33200.018563752</v>
       </c>
       <c r="I15" s="47" t="n">
         <f aca="false">SUM(I8:I14)</f>
@@ -1530,7 +1533,7 @@
       </c>
       <c r="J15" s="47" t="n">
         <f aca="false">SUM(J8:J14)</f>
-        <v>220303.988364379</v>
+        <v>211750.651884379</v>
       </c>
       <c r="K15" s="48"/>
       <c r="L15" s="48"/>
@@ -1634,7 +1637,7 @@
       </c>
       <c r="H19" s="35" t="n">
         <f aca="false">$B$19*H11</f>
-        <v>57.03364764864</v>
+        <v>28.51682382432</v>
       </c>
       <c r="I19" s="35" t="n">
         <f aca="false">$B$19*I11</f>
@@ -1642,7 +1645,7 @@
       </c>
       <c r="J19" s="35" t="n">
         <f aca="false">SUM(E19:I19)</f>
-        <v>293.391091082253</v>
+        <v>264.874267257933</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,15 +1704,15 @@
       </c>
       <c r="H21" s="55" t="n">
         <f aca="false">SUM(H17:H20)</f>
-        <v>1706.77886030696</v>
+        <v>1678.26203648264</v>
       </c>
       <c r="I21" s="55" t="n">
         <f aca="false">SUM(I17:I20)</f>
-        <v>1740.91443751311</v>
+        <v>1740.9144375131</v>
       </c>
       <c r="J21" s="55" t="n">
         <f aca="false">SUM(J17:J20)</f>
-        <v>9296.44580084246</v>
+        <v>9267.92897701814</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,7 +1748,7 @@
       </c>
       <c r="H23" s="47" t="n">
         <f aca="false">H15+H21</f>
-        <v>43460.133904059</v>
+        <v>34878.2806002346</v>
       </c>
       <c r="I23" s="47" t="n">
         <f aca="false">I15+I21</f>
@@ -1753,7 +1756,7 @@
       </c>
       <c r="J23" s="47" t="n">
         <f aca="false">J15+J21</f>
-        <v>229600.434165221</v>
+        <v>221018.580861397</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,7 +2400,8 @@
         <v>0</v>
       </c>
       <c r="J46" s="66" t="n">
-        <v>0</v>
+        <f aca="false">SUM(E46:I46)</f>
+        <v>2000</v>
       </c>
       <c r="K46" s="54"/>
     </row>
@@ -2406,69 +2410,69 @@
         <v>74</v>
       </c>
       <c r="B47" s="26" t="n">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="C47" s="72" t="n">
-        <v>2</v>
-      </c>
-      <c r="D47" s="72" t="s">
-        <v>70</v>
+        <v>3</v>
+      </c>
+      <c r="D47" s="72" t="n">
+        <v>1</v>
       </c>
       <c r="E47" s="66" t="n">
         <v>0</v>
       </c>
       <c r="F47" s="66" t="n">
-        <f aca="false">B47</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="G47" s="66" t="n">
-        <f aca="false">B47</f>
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="H47" s="66" t="n">
         <v>0</v>
       </c>
       <c r="I47" s="66" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J47" s="66" t="n">
         <f aca="false">SUM(E47:I47)</f>
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="K47" s="54"/>
     </row>
-    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="27" t="s">
         <v>75</v>
       </c>
       <c r="B48" s="26" t="n">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="C48" s="72" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" s="72" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D48" s="72" t="s">
+        <v>70</v>
       </c>
       <c r="E48" s="66" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F48" s="66" t="n">
-        <v>500</v>
+        <f aca="false">B48</f>
+        <v>2500</v>
       </c>
       <c r="G48" s="66" t="n">
-        <v>500</v>
+        <f aca="false">B48</f>
+        <v>2500</v>
       </c>
       <c r="H48" s="66" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I48" s="66" t="n">
-        <v>500</v>
+        <f aca="false">0</f>
+        <v>0</v>
       </c>
       <c r="J48" s="66" t="n">
         <f aca="false">SUM(E48:I48)</f>
-        <v>2500</v>
+        <v>6000</v>
       </c>
       <c r="K48" s="54"/>
     </row>
@@ -2477,269 +2481,293 @@
         <v>76</v>
       </c>
       <c r="B49" s="26" t="n">
+        <v>500</v>
+      </c>
+      <c r="C49" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="F49" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="G49" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="H49" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="I49" s="66" t="n">
+        <v>500</v>
+      </c>
+      <c r="J49" s="66" t="n">
+        <f aca="false">SUM(E49:I49)</f>
+        <v>2500</v>
+      </c>
+      <c r="K49" s="54"/>
+    </row>
+    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="26" t="n">
         <f aca="false">450+(2*250)+(3*74)+100</f>
         <v>1272</v>
       </c>
-      <c r="C49" s="72" t="n">
+      <c r="C50" s="72" t="n">
         <v>1</v>
       </c>
-      <c r="D49" s="72" t="n">
+      <c r="D50" s="72" t="n">
         <v>1</v>
       </c>
-      <c r="E49" s="66" t="n">
+      <c r="E50" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="F49" s="66" t="n">
+      <c r="F50" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="G49" s="66" t="n">
+      <c r="G50" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="H49" s="66" t="n">
+      <c r="H50" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="I49" s="66" t="n">
+      <c r="I50" s="66" t="n">
         <v>1272</v>
       </c>
-      <c r="J49" s="66" t="n">
-        <f aca="false">SUM(E49:I49)</f>
+      <c r="J50" s="66" t="n">
+        <f aca="false">SUM(E50:I50)</f>
         <v>6360</v>
       </c>
-      <c r="K49" s="54"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="47" t="n">
-        <f aca="false">SUM(E43:E49)</f>
+      <c r="K50" s="54"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="45"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="47" t="n">
+        <f aca="false">SUM(E43:E50)</f>
         <v>4442</v>
       </c>
-      <c r="F50" s="47" t="n">
-        <f aca="false">SUM(F43:F49)</f>
+      <c r="F51" s="47" t="n">
+        <f aca="false">SUM(F43:F50)</f>
         <v>9112</v>
       </c>
-      <c r="G50" s="47" t="n">
-        <f aca="false">SUM(G43:G49)</f>
-        <v>15452</v>
-      </c>
-      <c r="H50" s="47" t="n">
-        <f aca="false">SUM(H43:H49)</f>
-        <v>7582</v>
-      </c>
-      <c r="I50" s="47" t="n">
-        <f aca="false">SUM(I43:I49)</f>
-        <v>3472</v>
-      </c>
-      <c r="J50" s="47" t="n">
-        <f aca="false">SUM(J43:J49)</f>
-        <v>38060</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="85"/>
-      <c r="B51" s="86"/>
-      <c r="C51" s="86"/>
-      <c r="D51" s="87"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="66"/>
-      <c r="I51" s="66"/>
-      <c r="J51" s="66"/>
+      <c r="G51" s="47" t="n">
+        <f aca="false">SUM(G43:G50)</f>
+        <v>16452</v>
+      </c>
+      <c r="H51" s="47" t="n">
+        <f aca="false">SUM(H43:H50)</f>
+        <v>8582</v>
+      </c>
+      <c r="I51" s="47" t="n">
+        <f aca="false">SUM(I43:I50)</f>
+        <v>4472</v>
+      </c>
+      <c r="J51" s="47" t="n">
+        <f aca="false">SUM(J43:J50)</f>
+        <v>43060</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="88" t="s">
-        <v>78</v>
-      </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="89"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="47" t="n">
-        <f aca="false">E29+E38+E50</f>
+      <c r="A52" s="85"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="87"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="66"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="66"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="89"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="47" t="n">
+        <f aca="false">E29+E38+E51</f>
         <v>104442</v>
       </c>
-      <c r="F52" s="47" t="n">
-        <f aca="false">F29+F38+F50</f>
+      <c r="F53" s="47" t="n">
+        <f aca="false">F29+F38+F51</f>
         <v>25432</v>
       </c>
-      <c r="G52" s="47" t="n">
-        <f aca="false">G29+G38+G50</f>
-        <v>17900</v>
-      </c>
-      <c r="H52" s="47" t="n">
-        <f aca="false">H29+H38+H50</f>
-        <v>10078.96</v>
-      </c>
-      <c r="I52" s="47" t="n">
-        <f aca="false">I29+I38+I50</f>
-        <v>5988.2952</v>
-      </c>
-      <c r="J52" s="47" t="n">
-        <f aca="false">J29+J38+J50</f>
-        <v>161841.2552</v>
-      </c>
-      <c r="K52" s="91"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="92"/>
-      <c r="B53" s="93"/>
-      <c r="C53" s="93"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="95"/>
-      <c r="F53" s="95"/>
-      <c r="G53" s="95"/>
-      <c r="H53" s="95"/>
-      <c r="I53" s="95"/>
-      <c r="J53" s="58"/>
+      <c r="G53" s="47" t="n">
+        <f aca="false">G29+G38+G51</f>
+        <v>18900</v>
+      </c>
+      <c r="H53" s="47" t="n">
+        <f aca="false">H29+H38+H51</f>
+        <v>11078.96</v>
+      </c>
+      <c r="I53" s="47" t="n">
+        <f aca="false">I29+I38+I51</f>
+        <v>6988.2952</v>
+      </c>
+      <c r="J53" s="47" t="n">
+        <f aca="false">J29+J38+J51</f>
+        <v>166841.2552</v>
+      </c>
       <c r="K53" s="91"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" s="89"/>
-      <c r="C54" s="89"/>
-      <c r="D54" s="90"/>
-      <c r="E54" s="47" t="n">
-        <f aca="false">E23+E52</f>
+      <c r="A54" s="92"/>
+      <c r="B54" s="93"/>
+      <c r="C54" s="93"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="95"/>
+      <c r="F54" s="95"/>
+      <c r="G54" s="95"/>
+      <c r="H54" s="95"/>
+      <c r="I54" s="95"/>
+      <c r="J54" s="58"/>
+      <c r="K54" s="91"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="88" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="89"/>
+      <c r="C55" s="89"/>
+      <c r="D55" s="90"/>
+      <c r="E55" s="47" t="n">
+        <f aca="false">E23+E53</f>
         <v>151480.690416</v>
       </c>
-      <c r="F54" s="47" t="n">
-        <f aca="false">F23+F52</f>
+      <c r="F55" s="47" t="n">
+        <f aca="false">F23+F53</f>
         <v>71359.25033632</v>
       </c>
-      <c r="G54" s="47" t="n">
-        <f aca="false">G23+G52</f>
-        <v>66745.0229267024</v>
-      </c>
-      <c r="H54" s="47" t="n">
-        <f aca="false">H23+H52</f>
-        <v>53539.093904059</v>
-      </c>
-      <c r="I54" s="47" t="n">
-        <f aca="false">I23+I52</f>
-        <v>50317.6317821402</v>
-      </c>
-      <c r="J54" s="55" t="n">
-        <f aca="false">SUM(E54:I54)</f>
-        <v>393441.689365221</v>
-      </c>
-      <c r="K54" s="91"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="92"/>
-      <c r="B55" s="96" t="s">
+      <c r="G55" s="47" t="n">
+        <f aca="false">G23+G53</f>
+        <v>67745.0229267024</v>
+      </c>
+      <c r="H55" s="47" t="n">
+        <f aca="false">H23+H53</f>
+        <v>45957.2406002346</v>
+      </c>
+      <c r="I55" s="47" t="n">
+        <f aca="false">I23+I53</f>
+        <v>51317.6317821402</v>
+      </c>
+      <c r="J55" s="55" t="n">
+        <f aca="false">SUM(E55:I55)</f>
+        <v>387859.836061397</v>
+      </c>
+      <c r="K55" s="91"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="92"/>
+      <c r="B56" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="94"/>
-      <c r="E55" s="95"/>
-      <c r="F55" s="95"/>
-      <c r="G55" s="95"/>
-      <c r="H55" s="95"/>
-      <c r="I55" s="95"/>
-      <c r="J55" s="58"/>
-      <c r="K55" s="91"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="88" t="s">
+      <c r="C56" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="B56" s="97" t="n">
+      <c r="D56" s="94"/>
+      <c r="E56" s="95"/>
+      <c r="F56" s="95"/>
+      <c r="G56" s="95"/>
+      <c r="H56" s="95"/>
+      <c r="I56" s="95"/>
+      <c r="J56" s="58"/>
+      <c r="K56" s="91"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="97" t="n">
         <v>0.557</v>
       </c>
-      <c r="C56" s="98" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="90"/>
-      <c r="E56" s="47" t="n">
+      <c r="C57" s="98" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="90"/>
+      <c r="E57" s="47" t="n">
         <f aca="false">E15*0.557</f>
         <v>25054.21648</v>
       </c>
-      <c r="F56" s="47" t="n">
+      <c r="F57" s="47" t="n">
         <f aca="false">F15*0.557</f>
         <v>24658.8327036</v>
       </c>
-      <c r="G56" s="47" t="n">
+      <c r="G57" s="47" t="n">
         <f aca="false">G15*0.557</f>
         <v>26017.902441432</v>
       </c>
-      <c r="H56" s="47" t="n">
+      <c r="H57" s="47" t="n">
         <f aca="false">H15*0.557</f>
-        <v>23256.6187593699</v>
-      </c>
-      <c r="I56" s="47" t="n">
+        <v>18492.4103400099</v>
+      </c>
+      <c r="I57" s="47" t="n">
         <f aca="false">I15*0.557</f>
         <v>23721.7511345573</v>
       </c>
-      <c r="J56" s="55" t="n">
-        <f aca="false">SUM(E56:I56)</f>
-        <v>122709.321518959</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="92"/>
-      <c r="B57" s="99"/>
-      <c r="C57" s="93"/>
-      <c r="D57" s="94"/>
-      <c r="E57" s="95"/>
-      <c r="F57" s="95"/>
-      <c r="G57" s="95"/>
-      <c r="H57" s="95"/>
-      <c r="I57" s="95"/>
-      <c r="J57" s="58"/>
+      <c r="J57" s="55" t="n">
+        <f aca="false">SUM(E57:I57)</f>
+        <v>117945.113099599</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="100" t="s">
-        <v>83</v>
-      </c>
-      <c r="B58" s="101"/>
-      <c r="C58" s="101"/>
-      <c r="D58" s="102"/>
-      <c r="E58" s="103" t="n">
-        <f aca="false">E54+E56</f>
+      <c r="A58" s="92"/>
+      <c r="B58" s="99"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="94"/>
+      <c r="E58" s="95"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="95"/>
+      <c r="H58" s="95"/>
+      <c r="I58" s="95"/>
+      <c r="J58" s="58"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="101"/>
+      <c r="C59" s="101"/>
+      <c r="D59" s="102"/>
+      <c r="E59" s="103" t="n">
+        <f aca="false">E55+E57</f>
         <v>176534.906896</v>
       </c>
-      <c r="F58" s="103" t="n">
-        <f aca="false">F54+F56</f>
+      <c r="F59" s="103" t="n">
+        <f aca="false">F55+F57</f>
         <v>96018.08303992</v>
       </c>
-      <c r="G58" s="103" t="n">
-        <f aca="false">G54+G56</f>
-        <v>92762.9253681344</v>
-      </c>
-      <c r="H58" s="103" t="n">
-        <f aca="false">H54+H56</f>
-        <v>76795.7126634288</v>
-      </c>
-      <c r="I58" s="103" t="n">
-        <f aca="false">I54+I56</f>
-        <v>74039.3829166974</v>
-      </c>
-      <c r="J58" s="103" t="n">
-        <f aca="false">J54+J56</f>
-        <v>516151.010884181</v>
-      </c>
-      <c r="K58" s="91"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="104"/>
-      <c r="D59" s="105"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="54"/>
-      <c r="G59" s="54"/>
-      <c r="H59" s="54"/>
-      <c r="I59" s="54"/>
-      <c r="J59" s="54"/>
+      <c r="G59" s="103" t="n">
+        <f aca="false">G55+G57</f>
+        <v>93762.9253681344</v>
+      </c>
+      <c r="H59" s="103" t="n">
+        <f aca="false">H55+H57</f>
+        <v>64449.6509402445</v>
+      </c>
+      <c r="I59" s="103" t="n">
+        <f aca="false">I55+I57</f>
+        <v>75039.3829166974</v>
+      </c>
+      <c r="J59" s="103" t="n">
+        <f aca="false">J55+J57</f>
+        <v>505804.949160996</v>
+      </c>
+      <c r="K59" s="91"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="106"/>
+      <c r="A60" s="104"/>
       <c r="D60" s="105"/>
       <c r="E60" s="54"/>
       <c r="F60" s="54"/>
@@ -2748,7 +2776,16 @@
       <c r="I60" s="54"/>
       <c r="J60" s="54"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="106"/>
+      <c r="D61" s="105"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="54"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="54"/>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
@@ -2778,7 +2815,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
@@ -2786,7 +2823,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="107" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B1" s="108"/>
       <c r="C1" s="109"/>
@@ -2802,24 +2839,24 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="110" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B3" s="110" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" s="110" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D3" s="110" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E3" s="110" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="109" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B4" s="108" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
project plan update, corresponding budget updates
</commit_message>
<xml_diff>
--- a/NSF_Career Budget_Hanson.xlsx
+++ b/NSF_Career Budget_Hanson.xlsx
@@ -1120,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1423,16 +1423,16 @@
         <v>8621.06652</v>
       </c>
       <c r="H12" s="35" t="n">
-        <f aca="false">G12*1.02*0.33</f>
-        <v>2901.850990632</v>
+        <f aca="false">G12*1.02*0.67</f>
+        <v>5891.636859768</v>
       </c>
       <c r="I12" s="35" t="n">
-        <f aca="false">H12*1.02</f>
-        <v>2959.88801044464</v>
+        <f aca="false">H12*1.02*0</f>
+        <v>0</v>
       </c>
       <c r="J12" s="35" t="n">
         <f aca="false">SUM(E12:I12)</f>
-        <v>25670.1475210766</v>
+        <v>25700.045379768</v>
       </c>
     </row>
     <row r="13" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1525,15 +1525,15 @@
       </c>
       <c r="H15" s="47" t="n">
         <f aca="false">SUM(H8:H14)</f>
-        <v>33200.018563752</v>
+        <v>36189.804432888</v>
       </c>
       <c r="I15" s="47" t="n">
         <f aca="false">SUM(I8:I14)</f>
-        <v>42588.4221446271</v>
+        <v>39628.5341341824</v>
       </c>
       <c r="J15" s="47" t="n">
         <f aca="false">SUM(J8:J14)</f>
-        <v>211750.651884379</v>
+        <v>211780.54974307</v>
       </c>
       <c r="K15" s="48"/>
       <c r="L15" s="48"/>
@@ -1671,15 +1671,15 @@
       </c>
       <c r="H20" s="35" t="n">
         <f aca="false">H12*$D$20</f>
-        <v>231.567709052434</v>
+        <v>470.152621409487</v>
       </c>
       <c r="I20" s="35" t="n">
         <f aca="false">I12*$D$20</f>
-        <v>236.199063233482</v>
+        <v>0</v>
       </c>
       <c r="J20" s="35" t="n">
         <f aca="false">SUM(E20:I20)</f>
-        <v>2048.47777218192</v>
+        <v>2050.86362130549</v>
       </c>
       <c r="K20" s="54"/>
     </row>
@@ -1704,15 +1704,15 @@
       </c>
       <c r="H21" s="55" t="n">
         <f aca="false">SUM(H17:H20)</f>
-        <v>1678.26203648264</v>
+        <v>1916.8469488397</v>
       </c>
       <c r="I21" s="55" t="n">
         <f aca="false">SUM(I17:I20)</f>
-        <v>1740.9144375131</v>
+        <v>1504.71537427962</v>
       </c>
       <c r="J21" s="55" t="n">
         <f aca="false">SUM(J17:J20)</f>
-        <v>9267.92897701814</v>
+        <v>9270.31482614171</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,15 +1748,15 @@
       </c>
       <c r="H23" s="47" t="n">
         <f aca="false">H15+H21</f>
-        <v>34878.2806002346</v>
+        <v>38106.6513817277</v>
       </c>
       <c r="I23" s="47" t="n">
         <f aca="false">I15+I21</f>
-        <v>44329.3365821402</v>
+        <v>41133.249508462</v>
       </c>
       <c r="J23" s="47" t="n">
         <f aca="false">J15+J21</f>
-        <v>221018.580861397</v>
+        <v>221050.864569212</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2428,14 +2428,14 @@
         <v>1000</v>
       </c>
       <c r="H47" s="66" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I47" s="66" t="n">
         <v>1000</v>
       </c>
       <c r="J47" s="66" t="n">
         <f aca="false">SUM(E47:I47)</f>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="K47" s="54"/>
     </row>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="H51" s="47" t="n">
         <f aca="false">SUM(H43:H50)</f>
-        <v>8582</v>
+        <v>9582</v>
       </c>
       <c r="I51" s="47" t="n">
         <f aca="false">SUM(I43:I50)</f>
@@ -2574,7 +2574,7 @@
       </c>
       <c r="J51" s="47" t="n">
         <f aca="false">SUM(J43:J50)</f>
-        <v>43060</v>
+        <v>44060</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="H53" s="47" t="n">
         <f aca="false">H29+H38+H51</f>
-        <v>11078.96</v>
+        <v>12078.96</v>
       </c>
       <c r="I53" s="47" t="n">
         <f aca="false">I29+I38+I51</f>
@@ -2618,7 +2618,7 @@
       </c>
       <c r="J53" s="47" t="n">
         <f aca="false">J29+J38+J51</f>
-        <v>166841.2552</v>
+        <v>167841.2552</v>
       </c>
       <c r="K53" s="91"/>
     </row>
@@ -2656,15 +2656,15 @@
       </c>
       <c r="H55" s="47" t="n">
         <f aca="false">H23+H53</f>
-        <v>45957.2406002346</v>
+        <v>50185.6113817277</v>
       </c>
       <c r="I55" s="47" t="n">
         <f aca="false">I23+I53</f>
-        <v>51317.6317821402</v>
+        <v>48121.544708462</v>
       </c>
       <c r="J55" s="55" t="n">
         <f aca="false">SUM(E55:I55)</f>
-        <v>387859.836061397</v>
+        <v>388892.119769212</v>
       </c>
       <c r="K55" s="91"/>
     </row>
@@ -2710,15 +2710,15 @@
       </c>
       <c r="H57" s="47" t="n">
         <f aca="false">H15*0.557</f>
-        <v>18492.4103400099</v>
+        <v>20157.7210691186</v>
       </c>
       <c r="I57" s="47" t="n">
         <f aca="false">I15*0.557</f>
-        <v>23721.7511345573</v>
+        <v>22073.0935127396</v>
       </c>
       <c r="J57" s="55" t="n">
         <f aca="false">SUM(E57:I57)</f>
-        <v>117945.113099599</v>
+        <v>117961.76620689</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2754,15 +2754,15 @@
       </c>
       <c r="H59" s="103" t="n">
         <f aca="false">H55+H57</f>
-        <v>64449.6509402445</v>
+        <v>70343.3324508463</v>
       </c>
       <c r="I59" s="103" t="n">
         <f aca="false">I55+I57</f>
-        <v>75039.3829166974</v>
+        <v>70194.6382212016</v>
       </c>
       <c r="J59" s="103" t="n">
         <f aca="false">J55+J57</f>
-        <v>505804.949160996</v>
+        <v>506853.885976102</v>
       </c>
       <c r="K59" s="91"/>
     </row>
@@ -2815,7 +2815,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>

</xml_diff>